<commit_message>
Password reset pages part - 1
</commit_message>
<xml_diff>
--- a/site_map_details.xlsx
+++ b/site_map_details.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\GMIT\PROJECTS\ServerSideRad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\GMIT\PROJECTS\ServerSideRad\ASP.net-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -379,6 +379,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -390,9 +393,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -711,10 +711,10 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,7 +755,7 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
@@ -775,10 +775,10 @@
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="8" t="s">
         <v>32</v>
       </c>
       <c r="E3" t="s">
@@ -795,8 +795,8 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
       <c r="E4" t="s">
         <v>24</v>
       </c>
@@ -811,8 +811,8 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
       <c r="E5" t="s">
         <v>31</v>
       </c>
@@ -827,8 +827,8 @@
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8"/>
       <c r="E6" t="s">
         <v>29</v>
       </c>
@@ -918,7 +918,7 @@
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>26</v>
       </c>
       <c r="D11" t="s">
@@ -938,7 +938,7 @@
       <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="7"/>
       <c r="D12" t="s">
         <v>38</v>
       </c>
@@ -956,7 +956,7 @@
       <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="7"/>
       <c r="D13" t="s">
         <v>28</v>
       </c>
@@ -974,7 +974,7 @@
       <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="7"/>
       <c r="D14" t="s">
         <v>38</v>
       </c>
@@ -1097,7 +1097,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B2" t="s">
@@ -1108,7 +1108,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
+      <c r="A3" s="7"/>
       <c r="B3" t="s">
         <v>59</v>
       </c>
@@ -1117,7 +1117,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" t="s">
         <v>61</v>
       </c>
@@ -1126,7 +1126,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" t="s">
         <v>63</v>
       </c>
@@ -1135,7 +1135,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" t="s">
         <v>62</v>
       </c>
@@ -1144,7 +1144,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7"/>
       <c r="B7" t="s">
         <v>64</v>
       </c>
@@ -1153,7 +1153,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
+      <c r="A8" s="7"/>
       <c r="B8" t="s">
         <v>83</v>
       </c>
@@ -1162,7 +1162,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
+      <c r="A9" s="7"/>
       <c r="B9" t="s">
         <v>85</v>
       </c>
@@ -1178,7 +1178,7 @@
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>67</v>
       </c>
       <c r="B11" t="s">
@@ -1189,7 +1189,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
+      <c r="A12" s="7"/>
       <c r="B12" t="s">
         <v>69</v>
       </c>
@@ -1198,14 +1198,14 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="10" t="s">
         <v>70</v>
       </c>
       <c r="B14" t="s">
@@ -1216,7 +1216,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
+      <c r="A15" s="10"/>
       <c r="B15" t="s">
         <v>71</v>
       </c>
@@ -1225,14 +1225,14 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="7" t="s">
         <v>72</v>
       </c>
       <c r="B17" t="s">
@@ -1243,7 +1243,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
+      <c r="A18" s="7"/>
       <c r="B18" t="s">
         <v>68</v>
       </c>
@@ -1252,7 +1252,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
+      <c r="A19" s="7"/>
       <c r="B19" t="s">
         <v>73</v>
       </c>
@@ -1261,7 +1261,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
+      <c r="A20" s="7"/>
       <c r="B20" t="s">
         <v>74</v>
       </c>
@@ -1277,7 +1277,7 @@
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B22" t="s">
@@ -1288,7 +1288,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
+      <c r="A23" s="7"/>
       <c r="B23" t="s">
         <v>76</v>
       </c>
@@ -1297,7 +1297,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
+      <c r="A24" s="7"/>
       <c r="B24" t="s">
         <v>77</v>
       </c>
@@ -1306,7 +1306,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
+      <c r="A25" s="7"/>
       <c r="B25" t="s">
         <v>87</v>
       </c>
@@ -1315,7 +1315,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
+      <c r="A26" s="7"/>
       <c r="B26" t="s">
         <v>78</v>
       </c>
@@ -1324,7 +1324,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="6"/>
+      <c r="A27" s="7"/>
       <c r="B27" t="s">
         <v>79</v>
       </c>
@@ -1333,7 +1333,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="6"/>
+      <c r="A28" s="7"/>
       <c r="B28" t="s">
         <v>80</v>
       </c>
@@ -1342,7 +1342,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="6"/>
+      <c r="A29" s="7"/>
       <c r="B29" t="s">
         <v>81</v>
       </c>
@@ -1351,7 +1351,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="6"/>
+      <c r="A30" s="7"/>
       <c r="B30" t="s">
         <v>82</v>
       </c>
@@ -1367,7 +1367,7 @@
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="7" t="s">
         <v>88</v>
       </c>
       <c r="B32" t="s">
@@ -1378,7 +1378,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="6"/>
+      <c r="A33" s="7"/>
       <c r="B33" t="s">
         <v>89</v>
       </c>
@@ -1387,7 +1387,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="6"/>
+      <c r="A34" s="7"/>
       <c r="B34" t="s">
         <v>90</v>
       </c>
@@ -1396,7 +1396,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="6"/>
+      <c r="A35" s="7"/>
       <c r="B35" t="s">
         <v>85</v>
       </c>
@@ -1405,7 +1405,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="6"/>
+      <c r="A36" s="7"/>
       <c r="B36" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Site Map details updated
</commit_message>
<xml_diff>
--- a/site_map_details.xlsx
+++ b/site_map_details.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="99">
   <si>
     <t>Page</t>
   </si>
@@ -316,6 +316,12 @@
   </si>
   <si>
     <t>Pete</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Needs item image crud</t>
   </si>
 </sst>
 </file>
@@ -340,7 +346,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,6 +356,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -366,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -394,6 +406,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -708,13 +721,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD6"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,7 +741,7 @@
     <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -750,8 +763,11 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -768,7 +784,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -788,7 +804,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -804,39 +820,45 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="8"/>
-      <c r="E5" t="s">
+      <c r="E5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="11" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="H5" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8"/>
-      <c r="E6" t="s">
+      <c r="E6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="11" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -854,7 +876,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -871,7 +893,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -891,7 +913,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -911,7 +933,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -931,7 +953,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -949,7 +971,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -967,7 +989,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -985,7 +1007,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1002,7 +1024,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -1019,24 +1041,27 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="11" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Cart layout & cookie managment sorted with one time load and redirect...
</commit_message>
<xml_diff>
--- a/site_map_details.xlsx
+++ b/site_map_details.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="102">
   <si>
     <t>Page</t>
   </si>
@@ -322,13 +322,22 @@
   </si>
   <si>
     <t>Needs item image crud</t>
+  </si>
+  <si>
+    <t>Not persent</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Out of scope (The only adimn feature, would require admin CRUD)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,8 +354,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -365,6 +381,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -378,22 +400,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -406,7 +420,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -724,10 +748,10 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,225 +791,252 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="H2" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="4" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="H3" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="H4" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="11" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="H5" s="11" t="s">
+      <c r="G5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="11" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="9" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="H7" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="9" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="H8" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="H9" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="H10" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="9" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="H11" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="H12" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="4" t="s">
         <v>94</v>
       </c>
     </row>
@@ -996,7 +1047,7 @@
       <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="5"/>
       <c r="D14" t="s">
         <v>38</v>
       </c>
@@ -1007,21 +1058,24 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="3" t="s">
         <v>94</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1041,23 +1095,23 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H17" s="4" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1122,7 +1176,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B2" t="s">
@@ -1133,7 +1187,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
+      <c r="A3" s="5"/>
       <c r="B3" t="s">
         <v>59</v>
       </c>
@@ -1142,7 +1196,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
+      <c r="A4" s="5"/>
       <c r="B4" t="s">
         <v>61</v>
       </c>
@@ -1151,7 +1205,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
+      <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>63</v>
       </c>
@@ -1160,7 +1214,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
+      <c r="A6" s="5"/>
       <c r="B6" t="s">
         <v>62</v>
       </c>
@@ -1169,7 +1223,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
+      <c r="A7" s="5"/>
       <c r="B7" t="s">
         <v>64</v>
       </c>
@@ -1178,7 +1232,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
+      <c r="A8" s="5"/>
       <c r="B8" t="s">
         <v>83</v>
       </c>
@@ -1187,7 +1241,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>85</v>
       </c>
@@ -1196,14 +1250,14 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>67</v>
       </c>
       <c r="B11" t="s">
@@ -1214,7 +1268,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="5"/>
       <c r="B12" t="s">
         <v>69</v>
       </c>
@@ -1223,14 +1277,14 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="8" t="s">
         <v>70</v>
       </c>
       <c r="B14" t="s">
@@ -1241,7 +1295,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
+      <c r="A15" s="8"/>
       <c r="B15" t="s">
         <v>71</v>
       </c>
@@ -1250,14 +1304,14 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B17" t="s">
@@ -1268,7 +1322,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
+      <c r="A18" s="5"/>
       <c r="B18" t="s">
         <v>68</v>
       </c>
@@ -1277,7 +1331,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
+      <c r="A19" s="5"/>
       <c r="B19" t="s">
         <v>73</v>
       </c>
@@ -1286,7 +1340,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
+      <c r="A20" s="5"/>
       <c r="B20" t="s">
         <v>74</v>
       </c>
@@ -1295,14 +1349,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B22" t="s">
@@ -1313,7 +1367,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
+      <c r="A23" s="5"/>
       <c r="B23" t="s">
         <v>76</v>
       </c>
@@ -1322,7 +1376,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
+      <c r="A24" s="5"/>
       <c r="B24" t="s">
         <v>77</v>
       </c>
@@ -1331,7 +1385,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
+      <c r="A25" s="5"/>
       <c r="B25" t="s">
         <v>87</v>
       </c>
@@ -1340,7 +1394,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
+      <c r="A26" s="5"/>
       <c r="B26" t="s">
         <v>78</v>
       </c>
@@ -1349,7 +1403,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
+      <c r="A27" s="5"/>
       <c r="B27" t="s">
         <v>79</v>
       </c>
@@ -1358,7 +1412,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
+      <c r="A28" s="5"/>
       <c r="B28" t="s">
         <v>80</v>
       </c>
@@ -1367,7 +1421,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
+      <c r="A29" s="5"/>
       <c r="B29" t="s">
         <v>81</v>
       </c>
@@ -1376,7 +1430,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
+      <c r="A30" s="5"/>
       <c r="B30" t="s">
         <v>82</v>
       </c>
@@ -1385,14 +1439,14 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="5" t="s">
         <v>88</v>
       </c>
       <c r="B32" t="s">
@@ -1403,7 +1457,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
+      <c r="A33" s="5"/>
       <c r="B33" t="s">
         <v>89</v>
       </c>
@@ -1412,7 +1466,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
+      <c r="A34" s="5"/>
       <c r="B34" t="s">
         <v>90</v>
       </c>
@@ -1421,7 +1475,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
+      <c r="A35" s="5"/>
       <c r="B35" t="s">
         <v>85</v>
       </c>
@@ -1430,7 +1484,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
+      <c r="A36" s="5"/>
       <c r="B36" t="s">
         <v>83</v>
       </c>
@@ -1439,11 +1493,11 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
User list with single user privilege merged
</commit_message>
<xml_diff>
--- a/site_map_details.xlsx
+++ b/site_map_details.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="103">
   <si>
     <t>Page</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>Out of scope (The only adimn feature, would require admin CRUD)</t>
+  </si>
+  <si>
+    <t>Not present</t>
   </si>
 </sst>
 </file>
@@ -408,6 +411,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -419,17 +433,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -751,7 +754,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -795,7 +798,7 @@
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -818,10 +821,10 @@
       <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="11" t="s">
         <v>32</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -841,8 +844,8 @@
       <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="4" t="s">
         <v>24</v>
       </c>
@@ -860,8 +863,8 @@
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="4" t="s">
         <v>31</v>
       </c>
@@ -879,8 +882,8 @@
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="4" t="s">
         <v>29</v>
       </c>
@@ -891,44 +894,44 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="5" t="s">
         <v>99</v>
       </c>
     </row>
@@ -978,26 +981,26 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="5" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1008,7 +1011,7 @@
       <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="4" t="s">
         <v>38</v>
       </c>
@@ -1029,7 +1032,7 @@
       <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="4" t="s">
         <v>28</v>
       </c>
@@ -1039,23 +1042,29 @@
       <c r="G13" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="H13" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="5" t="s">
         <v>95</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -1078,21 +1087,24 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="5" t="s">
         <v>95</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1115,21 +1127,24 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="5" t="s">
         <v>95</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1176,7 +1191,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B2" t="s">
@@ -1187,7 +1202,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
+      <c r="A3" s="10"/>
       <c r="B3" t="s">
         <v>59</v>
       </c>
@@ -1196,7 +1211,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
+      <c r="A4" s="10"/>
       <c r="B4" t="s">
         <v>61</v>
       </c>
@@ -1205,7 +1220,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
+      <c r="A5" s="10"/>
       <c r="B5" t="s">
         <v>63</v>
       </c>
@@ -1214,7 +1229,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
+      <c r="A6" s="10"/>
       <c r="B6" t="s">
         <v>62</v>
       </c>
@@ -1223,7 +1238,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
+      <c r="A7" s="10"/>
       <c r="B7" t="s">
         <v>64</v>
       </c>
@@ -1232,7 +1247,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
+      <c r="A8" s="10"/>
       <c r="B8" t="s">
         <v>83</v>
       </c>
@@ -1241,7 +1256,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
+      <c r="A9" s="10"/>
       <c r="B9" t="s">
         <v>85</v>
       </c>
@@ -1257,7 +1272,7 @@
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="10" t="s">
         <v>67</v>
       </c>
       <c r="B11" t="s">
@@ -1268,7 +1283,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
+      <c r="A12" s="10"/>
       <c r="B12" t="s">
         <v>69</v>
       </c>
@@ -1277,14 +1292,14 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="13" t="s">
         <v>70</v>
       </c>
       <c r="B14" t="s">
@@ -1295,7 +1310,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
+      <c r="A15" s="13"/>
       <c r="B15" t="s">
         <v>71</v>
       </c>
@@ -1304,14 +1319,14 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="10" t="s">
         <v>72</v>
       </c>
       <c r="B17" t="s">
@@ -1322,7 +1337,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
+      <c r="A18" s="10"/>
       <c r="B18" t="s">
         <v>68</v>
       </c>
@@ -1331,7 +1346,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
+      <c r="A19" s="10"/>
       <c r="B19" t="s">
         <v>73</v>
       </c>
@@ -1340,7 +1355,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
+      <c r="A20" s="10"/>
       <c r="B20" t="s">
         <v>74</v>
       </c>
@@ -1356,7 +1371,7 @@
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B22" t="s">
@@ -1367,7 +1382,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
+      <c r="A23" s="10"/>
       <c r="B23" t="s">
         <v>76</v>
       </c>
@@ -1376,7 +1391,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
+      <c r="A24" s="10"/>
       <c r="B24" t="s">
         <v>77</v>
       </c>
@@ -1385,7 +1400,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
+      <c r="A25" s="10"/>
       <c r="B25" t="s">
         <v>87</v>
       </c>
@@ -1394,7 +1409,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
+      <c r="A26" s="10"/>
       <c r="B26" t="s">
         <v>78</v>
       </c>
@@ -1403,7 +1418,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
+      <c r="A27" s="10"/>
       <c r="B27" t="s">
         <v>79</v>
       </c>
@@ -1412,7 +1427,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
+      <c r="A28" s="10"/>
       <c r="B28" t="s">
         <v>80</v>
       </c>
@@ -1421,7 +1436,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
+      <c r="A29" s="10"/>
       <c r="B29" t="s">
         <v>81</v>
       </c>
@@ -1430,7 +1445,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
+      <c r="A30" s="10"/>
       <c r="B30" t="s">
         <v>82</v>
       </c>
@@ -1446,7 +1461,7 @@
       <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="10" t="s">
         <v>88</v>
       </c>
       <c r="B32" t="s">
@@ -1457,7 +1472,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
+      <c r="A33" s="10"/>
       <c r="B33" t="s">
         <v>89</v>
       </c>
@@ -1466,7 +1481,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
+      <c r="A34" s="10"/>
       <c r="B34" t="s">
         <v>90</v>
       </c>
@@ -1475,7 +1490,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="5"/>
+      <c r="A35" s="10"/>
       <c r="B35" t="s">
         <v>85</v>
       </c>
@@ -1484,7 +1499,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
+      <c r="A36" s="10"/>
       <c r="B36" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Store orders admin & all page styles
Css fixes, page titles etc.
</commit_message>
<xml_diff>
--- a/site_map_details.xlsx
+++ b/site_map_details.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="109">
   <si>
     <t>Page</t>
   </si>
@@ -150,9 +150,6 @@
     <t>The user can see the order history here.</t>
   </si>
   <si>
-    <t>Registered user list, should have links to User Crud</t>
-  </si>
-  <si>
     <t>User RUD</t>
   </si>
   <si>
@@ -174,9 +171,6 @@
     <t>Visitors should be able to send in support requests, imitating emails</t>
   </si>
   <si>
-    <t>List of orders with user list link (use store items layout)</t>
-  </si>
-  <si>
     <t>store_logs</t>
   </si>
   <si>
@@ -321,19 +315,43 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Needs item image crud</t>
-  </si>
-  <si>
     <t>Not persent</t>
   </si>
   <si>
     <t>Peter</t>
   </si>
   <si>
-    <t>Out of scope (The only adimn feature, would require admin CRUD)</t>
-  </si>
-  <si>
     <t>Not present</t>
+  </si>
+  <si>
+    <t>Store category search</t>
+  </si>
+  <si>
+    <t>All from footer</t>
+  </si>
+  <si>
+    <t>A brand or operating system based search with found items to display</t>
+  </si>
+  <si>
+    <t>Store item images</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>sore_items,  store_item_pictures</t>
+  </si>
+  <si>
+    <t>Selection of images for item details page/edits</t>
+  </si>
+  <si>
+    <t>Registered user list, should have links to User Crud (includes crud as Member not present)</t>
+  </si>
+  <si>
+    <t>Done not connected, so not functional</t>
+  </si>
+  <si>
+    <t>List of orders with user list link (use store items layout) (ADMIN)</t>
   </si>
 </sst>
 </file>
@@ -365,7 +383,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,6 +408,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -403,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -434,6 +458,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -748,13 +773,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -785,13 +810,13 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -808,10 +833,10 @@
         <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -831,10 +856,10 @@
         <v>23</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -850,10 +875,10 @@
         <v>24</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -869,10 +894,10 @@
         <v>31</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -888,31 +913,31 @@
         <v>29</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -929,10 +954,10 @@
         <v>33</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -952,204 +977,250 @@
         <v>34</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G11" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E14" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="B15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="5" t="s">
+      <c r="H18" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="D19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G19" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>102</v>
+      <c r="H20" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="C12:C15"/>
     <mergeCell ref="C3:C6"/>
     <mergeCell ref="D3:D6"/>
   </mergeCells>
@@ -1175,19 +1246,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1195,73 +1266,73 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
         <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1273,22 +1344,22 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1300,22 +1371,22 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1327,40 +1398,40 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1375,82 +1446,82 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1462,49 +1533,49 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C36" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Store item addition & javascript login/logout
</commit_message>
<xml_diff>
--- a/site_map_details.xlsx
+++ b/site_map_details.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="114">
   <si>
     <t>Page</t>
   </si>
@@ -177,9 +177,6 @@
     <t>Error logs for the store</t>
   </si>
   <si>
-    <t>CRUD for items, editing current items and/or adding new</t>
-  </si>
-  <si>
     <t>Technical requirements</t>
   </si>
   <si>
@@ -364,6 +361,12 @@
   </si>
   <si>
     <t>Simple sitemap naivagtion</t>
+  </si>
+  <si>
+    <t>NoLogin /admin</t>
+  </si>
+  <si>
+    <t>CRUD for items, editing current items and/or adding new trough item details</t>
   </si>
 </sst>
 </file>
@@ -788,10 +791,10 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -822,13 +825,13 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -845,10 +848,10 @@
         <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -868,10 +871,10 @@
         <v>23</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -887,10 +890,10 @@
         <v>24</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -906,10 +909,10 @@
         <v>31</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -925,10 +928,10 @@
         <v>29</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -946,10 +949,10 @@
         <v>47</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -957,7 +960,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>9</v>
+        <v>112</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>27</v>
@@ -966,10 +969,10 @@
         <v>33</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -989,33 +992,33 @@
         <v>34</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1035,10 +1038,10 @@
         <v>36</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1058,10 +1061,10 @@
         <v>39</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1079,10 +1082,10 @@
         <v>40</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1097,13 +1100,13 @@
         <v>28</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1121,10 +1124,10 @@
         <v>42</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -1138,13 +1141,13 @@
         <v>38</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1161,10 +1164,10 @@
         <v>45</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -1178,13 +1181,13 @@
         <v>27</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="G18" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -1201,56 +1204,56 @@
         <v>49</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="G20" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="E21" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>112</v>
-      </c>
       <c r="G21" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H21" s="10" t="s">
         <v>94</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1281,19 +1284,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
         <v>52</v>
-      </c>
-      <c r="C1" t="s">
-        <v>53</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1301,73 +1304,73 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
         <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
         <v>62</v>
-      </c>
-      <c r="C7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" t="s">
         <v>81</v>
-      </c>
-      <c r="C8" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
         <v>83</v>
-      </c>
-      <c r="C9" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1379,22 +1382,22 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
         <v>65</v>
       </c>
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1406,22 +1409,22 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
         <v>55</v>
-      </c>
-      <c r="C14" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1433,40 +1436,40 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
         <v>55</v>
-      </c>
-      <c r="C17" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" t="s">
         <v>72</v>
-      </c>
-      <c r="C20" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1481,82 +1484,82 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
         <v>55</v>
-      </c>
-      <c r="C22" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1568,49 +1571,49 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" t="s">
         <v>55</v>
-      </c>
-      <c r="C32" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
       <c r="B33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="11"/>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="11"/>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>